<commit_message>
updates for hackathon Nov 2/23
</commit_message>
<xml_diff>
--- a/data/data_digitization/occurrence_data/1_raw_data/HJ-5-occ-entry.xlsx
+++ b/data/data_digitization/occurrence_data/1_raw_data/HJ-5-occ-entry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/occurrence_data/1_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45BA867-FBD8-7146-B54D-AF33F58C6605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED03EB1C-58A8-4847-BE48-B8E1CD65A3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15340" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -2475,7 +2475,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>habitat</t>
   </si>
@@ -2631,6 +2631,15 @@
   </si>
   <si>
     <t>assColl</t>
+  </si>
+  <si>
+    <t>Thysanocarpus curvipes</t>
+  </si>
+  <si>
+    <t>Mayne Island</t>
+  </si>
+  <si>
+    <t>Mayne Island; cliffs facing navy channel</t>
   </si>
 </sst>
 </file>
@@ -2809,7 +2818,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3097,7 +3106,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3107,10 +3116,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3446,18 +3455,48 @@
       <c r="H7" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="L7"/>
       <c r="R7" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
+    <row r="8" spans="1:34" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="3">
+        <v>19750506</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="L8"/>
       <c r="AH8"/>
     </row>

</xml_diff>